<commit_message>
Refactor code formatting and add new SQL views and procedures for cosine similarity calculations
</commit_message>
<xml_diff>
--- a/Corpus de Google/Tablas.xlsx
+++ b/Corpus de Google/Tablas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\Documents\BDII_ProyectoFinal\Corpus de Google\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angel Josue Loayza Huarachi_UCSP\Semestre 5 - 2022 - CCOMP5\Base de datos II ♥♥♥\POYECTO FINAL GITHUB\Corpus de Google\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F80F249-B357-422B-A09D-C184B8EFB943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70F6B4A-4E53-451D-B58B-BB84698D384E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C6E252F9-F7F2-40D7-BDFA-2C282D4AD315}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>abba</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>raicesTable2</t>
+  </si>
+  <si>
+    <t>Continuacion…</t>
   </si>
 </sst>
 </file>
@@ -677,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1829EF-A684-4414-9FEC-EE003C15C8CF}">
-  <dimension ref="A2:H48"/>
+  <dimension ref="A2:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1147,6 +1150,11 @@
         <v>33</v>
       </c>
     </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="F13:H13"/>

</xml_diff>